<commit_message>
remove Count function from ExpressionResultLiteral and ExpressionResultNumeric
</commit_message>
<xml_diff>
--- a/helpers/membersOf_v2.xlsx
+++ b/helpers/membersOf_v2.xlsx
@@ -14,17 +14,66 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$158</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Valerii Reheda</author>
     <author>Valerii</author>
   </authors>
   <commentList>
-    <comment ref="E104" authorId="0">
+    <comment ref="E8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valerii Reheda:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+was ExpressionResultLiteral</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Valerii Reheda:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+was ExpressionResultNumeric</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E104" authorId="1">
       <text>
         <r>
           <rPr>
@@ -48,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F104" authorId="0">
+    <comment ref="F104" authorId="1">
       <text>
         <r>
           <rPr>
@@ -72,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E105" authorId="0">
+    <comment ref="E105" authorId="1">
       <text>
         <r>
           <rPr>
@@ -96,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F105" authorId="0">
+    <comment ref="F105" authorId="1">
       <text>
         <r>
           <rPr>
@@ -120,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E115" authorId="0">
+    <comment ref="E115" authorId="1">
       <text>
         <r>
           <rPr>
@@ -144,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F115" authorId="0">
+    <comment ref="F115" authorId="1">
       <text>
         <r>
           <rPr>
@@ -168,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E116" authorId="0">
+    <comment ref="E116" authorId="1">
       <text>
         <r>
           <rPr>
@@ -192,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F116" authorId="0">
+    <comment ref="F116" authorId="1">
       <text>
         <r>
           <rPr>
@@ -216,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E117" authorId="0">
+    <comment ref="E117" authorId="1">
       <text>
         <r>
           <rPr>
@@ -240,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F117" authorId="0">
+    <comment ref="F117" authorId="1">
       <text>
         <r>
           <rPr>
@@ -264,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E118" authorId="0">
+    <comment ref="E118" authorId="1">
       <text>
         <r>
           <rPr>
@@ -288,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F118" authorId="0">
+    <comment ref="F118" authorId="1">
       <text>
         <r>
           <rPr>
@@ -317,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="196">
   <si>
     <t>AltCats</t>
   </si>
@@ -1290,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G62" workbookViewId="0">
-      <selection activeCell="R86" sqref="R86:R88"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,12 +1757,8 @@
       <c r="D8" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="2" t="s">
         <v>132</v>
       </c>
@@ -1737,11 +1782,11 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="5"/>
-        <v>"ExpressionResultLiteral"</v>
+        <v>""</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="6"/>
-        <v>"ExpressionResultNumeric"</v>
+        <v>""</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="7"/>
@@ -1757,7 +1802,7 @@
       </c>
       <c r="R8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>functions.add(new Function("Count", "ExpressionResultNumeric", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "Specs"));</v>
+        <v>functions.add(new Function("Count", "ExpressionResultNumeric", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "Specs"));</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix Count, Height, Weight, Width, Value functions, check for double values
</commit_message>
<xml_diff>
--- a/helpers/membersOf_v2.xlsx
+++ b/helpers/membersOf_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="375" windowWidth="20115" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$158</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -265,54 +265,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E117" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Valerii:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-PdmMultivalueAttribute</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F117" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Valerii:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-PdmRepeatingAttribute</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="E118" authorId="1">
       <text>
         <r>
@@ -366,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="197">
   <si>
     <t>AltCats</t>
   </si>
@@ -954,6 +906,9 @@
   </si>
   <si>
     <t>GetPath()</t>
+  </si>
+  <si>
+    <t>NullableValueUnitPair</t>
   </si>
 </sst>
 </file>
@@ -1339,9 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7463,8 +7416,12 @@
       <c r="D117" t="s">
         <v>145</v>
       </c>
-      <c r="E117" s="6"/>
-      <c r="F117" s="4"/>
+      <c r="E117" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="G117" s="4" t="s">
         <v>178</v>
       </c>
@@ -7482,18 +7439,18 @@
       </c>
       <c r="M117" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="N117" t="str">
-        <f t="shared" si="15"/>
-        <v>""</v>
+        <f>CONCATENATE("""",F117,"""")</f>
+        <v>"NullableValueUnitPair"</v>
       </c>
       <c r="O117" t="str">
         <f t="shared" si="16"/>
         <v>"Gtin"</v>
       </c>
       <c r="P117" t="str">
-        <f t="shared" si="17"/>
+        <f>CONCATENATE("""",H117,"""")</f>
         <v>""</v>
       </c>
       <c r="Q117" t="str">
@@ -7502,7 +7459,7 @@
       </c>
       <c r="R117" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>functions.add(new Function("Value", "ExpressionResultLiteral", "PdmAttribute", "Gtin"));</v>
+        <v>functions.add(new Function("Value", "ExpressionResultLiteral", "PdmAttribute", "ExpressionResultNumeric", "NullableValueUnitPair", "Gtin"));</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
@@ -8721,6 +8678,9 @@
       <c r="D143" s="4" t="s">
         <v>127</v>
       </c>
+      <c r="E143" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="J143" s="5" t="str">
         <f t="shared" si="35"/>
         <v>"HasValue"</v>
@@ -8735,7 +8695,7 @@
       </c>
       <c r="M143" t="str">
         <f t="shared" si="38"/>
-        <v>""</v>
+        <v>"NullableValueUnitPair"</v>
       </c>
       <c r="N143" t="str">
         <f t="shared" si="39"/>
@@ -8755,7 +8715,7 @@
       </c>
       <c r="R143" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>functions.add(new Function("HasValue", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("HasValue", "ExpressionResultLiteral", "ExpressionResultNumeric", "NullableValueUnitPair"));</v>
       </c>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
@@ -8763,7 +8723,7 @@
         <v>181</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>184</v>
@@ -8774,7 +8734,7 @@
       </c>
       <c r="K144" t="str">
         <f t="shared" si="36"/>
-        <v>"ExpressionResultNumeric"</v>
+        <v>"NullableValueUnitPair"</v>
       </c>
       <c r="L144" t="str">
         <f t="shared" si="37"/>
@@ -8802,7 +8762,7 @@
       </c>
       <c r="R144" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>functions.add(new Function("Height", "ExpressionResultNumeric", "ProductPackage"));</v>
+        <v>functions.add(new Function("Height", "NullableValueUnitPair", "ProductPackage"));</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
@@ -8810,7 +8770,7 @@
         <v>182</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>184</v>
@@ -8821,7 +8781,7 @@
       </c>
       <c r="K145" t="str">
         <f t="shared" ref="K145:K151" si="42">CONCATENATE("""",B145,"""")</f>
-        <v>"ExpressionResultNumeric"</v>
+        <v>"NullableValueUnitPair"</v>
       </c>
       <c r="L145" t="str">
         <f t="shared" ref="L145:L150" si="43">CONCATENATE("""",D145,"""")</f>
@@ -8849,7 +8809,7 @@
       </c>
       <c r="R145" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>functions.add(new Function("Width", "ExpressionResultNumeric", "ProductPackage"));</v>
+        <v>functions.add(new Function("Width", "NullableValueUnitPair", "ProductPackage"));</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
@@ -8857,7 +8817,7 @@
         <v>183</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>184</v>
@@ -8868,7 +8828,7 @@
       </c>
       <c r="K146" t="str">
         <f t="shared" si="42"/>
-        <v>"ExpressionResultNumeric"</v>
+        <v>"NullableValueUnitPair"</v>
       </c>
       <c r="L146" t="str">
         <f t="shared" si="43"/>
@@ -8896,7 +8856,7 @@
       </c>
       <c r="R146" s="7" t="str">
         <f t="shared" si="19"/>
-        <v>functions.add(new Function("Weight", "ExpressionResultNumeric", "ProductPackage"));</v>
+        <v>functions.add(new Function("Weight", "NullableValueUnitPair", "ProductPackage"));</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
@@ -9467,7 +9427,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H158"/>
+  <autoFilter ref="A1:T158"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
fix issue with invoking Split function on ExpressionResultList
</commit_message>
<xml_diff>
--- a/helpers/membersOf_v2.xlsx
+++ b/helpers/membersOf_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="375" windowWidth="20115" windowHeight="7695"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$158</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -70,6 +70,30 @@
           </rPr>
           <t xml:space="preserve">
 was ExpressionResultNumeric</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D49" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+was: ExpressionResultList</t>
         </r>
       </text>
     </comment>
@@ -318,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="197">
   <si>
     <t>AltCats</t>
   </si>
@@ -915,7 +939,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -935,6 +959,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1294,7 +1331,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K37" workbookViewId="0">
+      <selection activeCell="R49" sqref="R49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3882,9 +3921,7 @@
       <c r="C49" t="s">
         <v>160</v>
       </c>
-      <c r="D49" t="s">
-        <v>126</v>
-      </c>
+      <c r="D49" s="4"/>
       <c r="E49" s="2" t="s">
         <v>128</v>
       </c>
@@ -3901,7 +3938,7 @@
       </c>
       <c r="L49" t="str">
         <f t="shared" si="4"/>
-        <v>"ExpressionResultList"</v>
+        <v>""</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="5"/>
@@ -3925,7 +3962,7 @@
       </c>
       <c r="R49" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>functions.add(new Function("Split()", "ExpressionResultList", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("Split()", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add Sum function to check
</commit_message>
<xml_diff>
--- a/helpers/membersOf_v2.xlsx
+++ b/helpers/membersOf_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="375" windowWidth="20115" windowHeight="7695"/>
@@ -12,9 +12,9 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$159</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -81,7 +81,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Valerii:</t>
         </r>
@@ -90,7 +90,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 was: ExpressionResultList</t>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="198">
   <si>
     <t>AltCats</t>
   </si>
@@ -933,13 +933,16 @@
   </si>
   <si>
     <t>NullableValueUnitPair</t>
+  </si>
+  <si>
+    <t>Sum()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -959,19 +962,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1329,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T158"/>
+  <dimension ref="A1:T159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K37" workbookViewId="0">
-      <selection activeCell="R49" sqref="R49"/>
+    <sheetView tabSelected="1" topLeftCell="G143" workbookViewId="0">
+      <selection activeCell="R159" sqref="R159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9289,7 +9279,7 @@
         <v>158</v>
       </c>
       <c r="J155" s="5" t="str">
-        <f t="shared" ref="J155:J158" si="59">CONCATENATE("""",A155,"""")</f>
+        <f t="shared" ref="J155:J159" si="59">CONCATENATE("""",A155,"""")</f>
         <v>"ToString()"</v>
       </c>
       <c r="K155" t="str">
@@ -9463,8 +9453,58 @@
         <v>functions.add(new Function("CategoryCode", "ExpressionResultLiteral", "Sku"));</v>
       </c>
     </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C159" t="s">
+        <v>160</v>
+      </c>
+      <c r="D159" t="s">
+        <v>126</v>
+      </c>
+      <c r="J159" s="5" t="str">
+        <f t="shared" si="59"/>
+        <v>"Sum()"</v>
+      </c>
+      <c r="K159" t="str">
+        <f t="shared" ref="K159" si="86">CONCATENATE("""",B159,"""")</f>
+        <v>"ExpressionResultNumeric"</v>
+      </c>
+      <c r="L159" t="str">
+        <f t="shared" ref="L159" si="87">CONCATENATE("""",D159,"""")</f>
+        <v>"ExpressionResultList"</v>
+      </c>
+      <c r="M159" t="str">
+        <f t="shared" ref="M159" si="88">CONCATENATE("""",E159,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N159" t="str">
+        <f t="shared" ref="N159" si="89">CONCATENATE("""",F159,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O159" t="str">
+        <f t="shared" ref="O159" si="90">CONCATENATE("""",G159,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P159" t="str">
+        <f t="shared" ref="P159" si="91">CONCATENATE("""",H159,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="Q159" t="str">
+        <f t="shared" ref="Q159" si="92">CONCATENATE("""",I159,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="R159" s="7" t="str">
+        <f t="shared" ref="R159" si="93">SUBSTITUTE(CONCATENATE($S$1,J159,$R$1,K159,$R$1,L159,$R$1,M159,$R$1,N159,$R$1,O159,$R$1,P159,$R$1,Q159,$T$1),", """"","")</f>
+        <v>functions.add(new Function("Sum()", "ExpressionResultNumeric", "ExpressionResultList"));</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:T158"/>
+  <autoFilter ref="A1:T159"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>